<commit_message>
Adding PF graphics 180304
</commit_message>
<xml_diff>
--- a/special-ed-income/special-ed-income.xlsx
+++ b/special-ed-income/special-ed-income.xlsx
@@ -14,10 +14,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
-    <t>label</t>
+    <t>key</t>
   </si>
   <si>
-    <t>key</t>
+    <t>label</t>
   </si>
   <si>
     <t>value</t>
@@ -68,13 +68,13 @@
     <t>Less than 50%</t>
   </si>
   <si>
+    <t>footnote</t>
+  </si>
+  <si>
     <t>15531.77</t>
   </si>
   <si>
     <t>&lt; 50%</t>
-  </si>
-  <si>
-    <t>footnote</t>
   </si>
   <si>
     <t>Low income categories are based on percentages of students who receive free and reduced lunch. CPS' free and reduced lunch average is about 80 percent.</t>
@@ -101,10 +101,10 @@
     </font>
     <font>
       <b/>
+      <sz val="14.0"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
     </font>
     <font>
       <sz val="14.0"/>
@@ -165,16 +165,16 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -203,11 +203,11 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -222,10 +222,10 @@
   </cols>
   <sheetData>
     <row r="1" ht="33.0" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="3"/>
@@ -317,7 +317,7 @@
     </row>
     <row r="4" ht="33.0" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
@@ -704,13 +704,13 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="4"/>
@@ -784,10 +784,10 @@
         <v>17</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">

</xml_diff>